<commit_message>
adding regression model, finish formatting
</commit_message>
<xml_diff>
--- a/raw_data/social_immigrants/english_by_country.xlsx
+++ b/raw_data/social_immigrants/english_by_country.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mengxi/Dropbox/MDE/Fall 2019/Data Gov1005/Projects/final_project/US-Immigration-Explorer/raw_data/social_immigrants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E746380-A08E-544D-ADAC-93233883AF37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6D975F-B072-D84B-A474-BE7B86CEEF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22420" yWindow="2020" windowWidth="28040" windowHeight="16580" xr2:uid="{E1D85367-B32D-DD4C-A733-E63E38B3C688}"/>
+    <workbookView xWindow="22420" yWindow="2020" windowWidth="28040" windowHeight="16580" activeTab="2" xr2:uid="{E1D85367-B32D-DD4C-A733-E63E38B3C688}"/>
   </bookViews>
   <sheets>
     <sheet name="English Speakling Capability" sheetId="2" r:id="rId1"/>
@@ -181,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -207,6 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10AE8D3-DFEA-3245-AE4A-E556B82D1BD4}">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
@@ -3353,10 +3354,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237FDB4F-CF56-4443-855E-8AE53E61765E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3365,7 +3366,7 @@
     <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -3373,7 +3374,7 @@
         <v>3075211124</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -3381,21 +3382,29 @@
         <v>0.91659999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="24">
         <v>3.6999999999999998E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="25">
+        <f>1-B3</f>
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="12">
         <f>1-63.4%</f>
         <v>0.36599999999999999</v>
+      </c>
+      <c r="C4" s="25">
+        <f>1-B4</f>
+        <v>0.63400000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>